<commit_message>
Group for LDAP integration
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-is/src/main/resources/plugin/is/oob/data/is.integration.zero.xlsx
+++ b/vertx-pin/zero-is/src/main/resources/plugin/is/oob/data/is.integration.zero.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/vertx-zero/vertx-pin/zero-is/src/main/resources/plugin/is/oob/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/lm/r14tlhyj7fncnytfwf3v8dc00000gn/T/tmp-12514-OO7Ztv2QHmXx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83994AB7-DFFC-C841-B4E6-6A82ADB04966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EB6E7E-E965-D049-A9D0-51760AE55EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="7080" windowWidth="33660" windowHeight="13860" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="74480" yWindow="-2900" windowWidth="33660" windowHeight="13860" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-CDATA" sheetId="7" r:id="rId1"/>
@@ -57,18 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4443b6d1-f9fa-41f6-a3ed-c1ec62fd12a5</t>
-  </si>
-  <si>
-    <t>e181e7a7-55ce-4a53-9e70-34dbd9e9ecdb</t>
-  </si>
-  <si>
-    <t>9908e33a-a22e-4bbc-90bd-04fa79396f08</t>
-  </si>
-  <si>
-    <t>a04bb496-3a3c-425f-ade8-ab488eb12458</t>
-  </si>
-  <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -258,9 +246,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>be686920-099e-4bd3-bb4c-185d088f0c53</t>
-  </si>
-  <si>
     <t>uid=admin,ou=system</t>
   </si>
   <si>
@@ -278,6 +263,21 @@
   <si>
     <t>集成详细配置（五种，测试专用）</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6160dfe6-47f1-484e-8502-2ff974b5ce82</t>
+  </si>
+  <si>
+    <t>e7dc12e2-c8a9-445e-945a-27bb108bb4c3</t>
+  </si>
+  <si>
+    <t>3f6762af-ca7a-40a2-b426-f39f1693dbb2</t>
+  </si>
+  <si>
+    <t>5793f209-5424-4d7a-8dd7-1d8d2b3bd8e9</t>
+  </si>
+  <si>
+    <t>f3912644-3a4b-4877-ba55-503e6bacacfd</t>
   </si>
 </sst>
 </file>
@@ -421,12 +421,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,6 +450,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -776,23 +776,23 @@
   <dimension ref="A2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="54.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="54.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
@@ -802,248 +802,248 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>42</v>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="A5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="10">
         <v>1024</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>47</v>
+      <c r="F5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="A6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="10">
         <v>80</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="A7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="10">
         <v>21</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="F7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>47</v>
+      <c r="K7" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="A8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="10">
         <v>25</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>47</v>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="10">
+        <v>10389</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="K9" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="12">
-        <v>10389</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>